<commit_message>
doc(Journal de travail) Ajout heures de journal de travail du 28.11.2024
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BotteauMathis.xlsx
+++ b/docs/Journal-de-Travail_BotteauMathis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutSehll\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4723AD-7F6D-4A66-8095-F32A6BB92317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6AEFE9-66D4-445C-BE9B-EB834FB172C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">Disscussion avec Mathis quant au projet a faire et les exigences de celui-ci </t>
+  </si>
+  <si>
+    <t>Création des users Storie et technical storie pour le projet (Installation Teams, Installation VisualStuioCode, Ajout au groupe docker, Message d'erreur, Message de validation, Test unitaires)</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1155,7 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2086,7 +2089,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2139,7 +2142,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 15 minutes</v>
+        <v>0 jours 2 heurs 15 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2154,7 +2157,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2162,7 +2165,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2216,16 +2219,24 @@
       </c>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="str">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
         <v/>
       </c>
       <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="37"/>
+      <c r="C8" s="48">
+        <v>2</v>
+      </c>
+      <c r="D8" s="49">
+        <v>0</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="M8" t="s">
         <v>3</v>
@@ -8708,7 +8719,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
@@ -8720,7 +8731,7 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -8847,7 +8858,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>1.0416666666666666E-2</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8870,17 +8881,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9103,6 +9103,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9112,17 +9123,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9139,4 +9139,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
web(backend): Lancement de lîndex.html comme page pour le backend
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BotteauMathis.xlsx
+++ b/docs/Journal-de-Travail_BotteauMathis.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3555D380-3262-4372-8807-896A492C00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE6F5F6-6176-41EB-8794-6B36B1CC63EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ecriture de la partie développement et conclusion du rapport </t>
+  </si>
+  <si>
+    <t>Création du site web frontend / backend de téléchargement du sccript. Création d'une db, connexion de la db au backend, connexion du frontend au backend, résoution problèmes de conversion des binaires au format string</t>
   </si>
 </sst>
 </file>
@@ -499,80 +502,6 @@
   <dxfs count="33">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -739,6 +668,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1250,7 +1253,7 @@
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3333333333333329E-2</c:v>
+                  <c:v>0.17708333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1974,18 +1977,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2180,8 +2183,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2234,7 +2237,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 15 minutes</v>
+        <v>0 jours 9 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2249,15 +2252,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>435</v>
+        <v>570</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2491,16 +2494,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+    <row r="14" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="37"/>
+        <v>50</v>
+      </c>
+      <c r="B14" s="47">
+        <v>45638</v>
+      </c>
+      <c r="C14" s="48">
+        <v>2</v>
+      </c>
+      <c r="D14" s="49">
+        <v>15</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -8805,28 +8818,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E13="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E13="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E13="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E13="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E13="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E13="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E13="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>$E13="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8901,11 +8914,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8913,7 +8926,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.17708333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9022,7 +9035,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.30208333333333331</v>
+        <v>0.39583333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9045,6 +9058,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9267,17 +9291,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9287,6 +9300,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9303,15 +9327,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): Ajout des heures de travail du 18.12.2024
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BotteauMathis.xlsx
+++ b/docs/Journal-de-Travail_BotteauMathis.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE6F5F6-6176-41EB-8794-6B36B1CC63EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF295A9A-B9C4-475F-B384-EAFBF26D4338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Création du site web frontend / backend de téléchargement du sccript. Création d'une db, connexion de la db au backend, connexion du frontend au backend, résoution problèmes de conversion des binaires au format string</t>
+  </si>
+  <si>
+    <t>Déployement sur azure, problèmes azure ne récupere pas l'application afin d'y accéder</t>
+  </si>
+  <si>
+    <t>Retour sur l'evaluation portfolio avec le professeur</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1259,7 @@
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17708333333333334</c:v>
+                  <c:v>0.28125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1262,7 +1268,7 @@
                   <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2183,8 +2189,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2237,7 +2243,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 30 minutes</v>
+        <v>0 jours 12 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2252,15 +2258,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>570</v>
+        <v>750</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2526,15 +2532,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="str">
+      <c r="A15" s="17">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="37"/>
+        <v>51</v>
+      </c>
+      <c r="B15" s="51">
+        <v>45644</v>
+      </c>
+      <c r="C15" s="52">
+        <v>2</v>
+      </c>
+      <c r="D15" s="53">
+        <v>30</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -2547,15 +2563,23 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="47"/>
+        <v>51</v>
+      </c>
+      <c r="B16" s="47">
+        <v>45644</v>
+      </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="37"/>
+      <c r="D16" s="49">
+        <v>30</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>39</v>
+      </c>
       <c r="G16" s="16"/>
       <c r="O16">
         <v>40</v>
@@ -8914,11 +8938,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8926,7 +8950,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.17708333333333334</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8972,7 +8996,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8980,7 +9004,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9035,7 +9059,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.39583333333333337</v>
+        <v>0.52083333333333326</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9058,17 +9082,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9291,6 +9304,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9300,17 +9324,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9327,4 +9340,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): Mise a jour des journaux de travaux / séparation
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_BotteauMathis.xlsx
+++ b/docs/Journal-de-Travail_BotteauMathis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd47qky\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF295A9A-B9C4-475F-B384-EAFBF26D4338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5B23E-DE03-4A26-9D2C-F09CAFA95DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -152,15 +152,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ecriture de la partie développement et conclusion du rapport </t>
-  </si>
-  <si>
-    <t>Création du site web frontend / backend de téléchargement du sccript. Création d'une db, connexion de la db au backend, connexion du frontend au backend, résoution problèmes de conversion des binaires au format string</t>
-  </si>
-  <si>
-    <t>Déployement sur azure, problèmes azure ne récupere pas l'application afin d'y accéder</t>
-  </si>
-  <si>
-    <t>Retour sur l'evaluation portfolio avec le professeur</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1250,7 @@
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28125</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1268,7 +1259,7 @@
                   <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2190,7 +2181,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2234,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 12 heurs 30 minutes</v>
+        <v>0 jours 7 heurs 15 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2258,15 +2249,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>300</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>750</v>
+        <v>435</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2500,26 +2491,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="str">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v>50</v>
-      </c>
-      <c r="B14" s="47">
-        <v>45638</v>
-      </c>
-      <c r="C14" s="48">
-        <v>2</v>
-      </c>
-      <c r="D14" s="49">
-        <v>15</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="37" t="s">
-        <v>37</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2532,25 +2513,15 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="17" t="str">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v>51</v>
-      </c>
-      <c r="B15" s="51">
-        <v>45644</v>
-      </c>
-      <c r="C15" s="52">
-        <v>2</v>
-      </c>
-      <c r="D15" s="53">
-        <v>30</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>38</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="18"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -2563,23 +2534,15 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="8" t="str">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v>51</v>
-      </c>
-      <c r="B16" s="47">
-        <v>45644</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B16" s="47"/>
       <c r="C16" s="48"/>
-      <c r="D16" s="49">
-        <v>30</v>
-      </c>
-      <c r="E16" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>39</v>
-      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="16"/>
       <c r="O16">
         <v>40</v>
@@ -8938,11 +8901,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8950,7 +8913,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.28125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8996,7 +8959,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9004,7 +8967,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9059,7 +9022,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.52083333333333326</v>
+        <v>0.30208333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9082,6 +9045,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9304,17 +9278,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9324,6 +9287,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9340,15 +9314,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>